<commit_message>
Added parameter-decoder to raspberry
</commit_message>
<xml_diff>
--- a/doc/SPI-Protokoll.xlsx
+++ b/doc/SPI-Protokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klosskopf\Desktop\Arbeit\Messbox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016E7AD9-3A41-4C05-8606-987DAF65E903}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6606A9-FDB9-4223-8F04-EC8F5EDCA774}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>0x02</t>
   </si>
   <si>
-    <t>nummer, wert</t>
-  </si>
-  <si>
     <t>get_daten</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>0x07</t>
   </si>
   <si>
-    <t>nummer,name,typ{s/f},parametrierbar{l/f/n},min,max,plotbar{y/n},(wahl1,wahl2,...);nummer,name,typ{s/f} …</t>
-  </si>
-  <si>
     <t>set_sample_freq</t>
   </si>
   <si>
@@ -184,6 +178,12 @@
   </si>
   <si>
     <t>Vin[4B]</t>
+  </si>
+  <si>
+    <t>kartenname,name,typ(s/f),parametrierbar(l/f/n),min,max,plotbar(y/n){wahl1,wahl2,…};name,typ(s/f) …</t>
+  </si>
+  <si>
+    <t>name, wert</t>
   </si>
 </sst>
 </file>
@@ -454,6 +454,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -464,11 +491,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -481,47 +514,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -806,7 +806,7 @@
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,27 +818,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="33"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="43"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="1"/>
@@ -846,8 +846,8 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
-        <v>21</v>
+      <c r="A2" s="44" t="s">
+        <v>20</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>9</v>
@@ -892,8 +892,8 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
@@ -901,18 +901,18 @@
         <v>6</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="37"/>
+        <v>17</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="48"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="2"/>
@@ -940,10 +940,10 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -953,18 +953,18 @@
         <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="35"/>
+        <v>17</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="46"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="2"/>
@@ -972,8 +972,8 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1034,20 +1034,20 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="39" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>6</v>
@@ -1080,8 +1080,8 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1092,28 +1092,28 @@
         <v>6</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="I9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="K9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="L9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="13" t="s">
-        <v>33</v>
-      </c>
       <c r="M9" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
@@ -1141,17 +1141,17 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>24</v>
+      <c r="A11" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="11"/>
@@ -1169,8 +1169,8 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1213,17 +1213,17 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="30" t="s">
-        <v>25</v>
+      <c r="A14" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1241,8 +1241,8 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="42"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="28"/>
       <c r="C16" s="5"/>
       <c r="D16" s="23"/>
@@ -1285,20 +1285,20 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>38</v>
+      <c r="A17" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="35" t="s">
         <v>41</v>
-      </c>
-      <c r="E17" s="49" t="s">
-        <v>43</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -1315,12 +1315,12 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="29"/>
-      <c r="B18" s="31"/>
+      <c r="A18" s="38"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="14" t="s">
@@ -1341,7 +1341,7 @@
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="42"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="28"/>
       <c r="C19" s="5"/>
       <c r="D19" s="23"/>
@@ -1361,17 +1361,17 @@
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>40</v>
+      <c r="A20" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="48" t="s">
-        <v>42</v>
+      <c r="D20" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>6</v>
@@ -1401,31 +1401,31 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="43"/>
-      <c r="B21" s="39"/>
+      <c r="A21" s="49"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="50" t="s">
+      <c r="D21" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="50" t="s">
+      <c r="H21" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="50" t="s">
+      <c r="I21" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="50" t="s">
+      <c r="J21" s="37" t="s">
         <v>47</v>
-      </c>
-      <c r="I21" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="51" t="s">
-        <v>49</v>
       </c>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
@@ -1454,10 +1454,10 @@
     </row>
     <row r="23" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>16</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>17</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="11"/>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="24" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="21" t="s">
         <v>26</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>27</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="11"/>

</xml_diff>

<commit_message>
Added rest of protokoll in post
</commit_message>
<xml_diff>
--- a/doc/SPI-Protokoll.xlsx
+++ b/doc/SPI-Protokoll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klosskopf\Desktop\Arbeit\Messbox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6606A9-FDB9-4223-8F04-EC8F5EDCA774}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44CFD7F-8E00-4D9D-A8F3-FD32F800A8FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-7650" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
   <si>
     <t>Befehl</t>
   </si>
@@ -180,10 +180,10 @@
     <t>Vin[4B]</t>
   </si>
   <si>
-    <t>kartenname,name,typ(s/f),parametrierbar(l/f/n),min,max,plotbar(y/n){wahl1,wahl2,…};name,typ(s/f) …</t>
-  </si>
-  <si>
-    <t>name, wert</t>
+    <t>wert</t>
+  </si>
+  <si>
+    <t>kartenname,nummer,name,typ(s/f),parametrierbar(l/f/n),min,max,plotbar(y/n){wahl1,wahl2,…};name,typ(s/f) …</t>
   </si>
 </sst>
 </file>
@@ -372,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -484,9 +484,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -514,14 +523,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,18 +830,18 @@
       <c r="C1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="43"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="46"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="1"/>
@@ -846,10 +849,10 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="44" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -893,7 +896,7 @@
     </row>
     <row r="3" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
@@ -903,16 +906,16 @@
       <c r="E3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="48"/>
+      <c r="F3" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="51"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="2"/>
@@ -943,7 +946,7 @@
       <c r="A5" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="43" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -955,16 +958,18 @@
       <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="46"/>
+      <c r="F5" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="49"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="2"/>
@@ -973,7 +978,7 @@
     </row>
     <row r="6" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38"/>
-      <c r="B6" s="40"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1037,7 +1042,7 @@
       <c r="A8" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="40" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1081,7 +1086,7 @@
     </row>
     <row r="9" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="38"/>
-      <c r="B9" s="40"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1141,10 +1146,10 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="40" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1169,8 +1174,8 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
-      <c r="B12" s="39"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1213,10 +1218,10 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="40" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -1241,8 +1246,8 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
-      <c r="B15" s="40"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1285,10 +1290,10 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="40" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="5" t="s">
@@ -1315,8 +1320,8 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="43"/>
       <c r="C18" s="5" t="s">
         <v>4</v>
       </c>
@@ -1364,7 +1369,7 @@
       <c r="A20" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="40" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1401,8 +1406,8 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="39"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="6" t="s">
         <v>4</v>
       </c>
@@ -1617,6 +1622,15 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D1:M1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F3:M3"/>
+    <mergeCell ref="G5:M5"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="A14:A15"/>
@@ -1625,15 +1639,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D1:M1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:M5"/>
-    <mergeCell ref="F3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactored fake SPI, add get_daten, get_status, draw graph in qt thread
</commit_message>
<xml_diff>
--- a/doc/SPI-Protokoll.xlsx
+++ b/doc/SPI-Protokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klosskopf\Desktop\Arbeit\Messbox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44CFD7F-8E00-4D9D-A8F3-FD32F800A8FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7416D5-DBEC-4744-8E06-A5CD2C73BABA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7650" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,21 +481,15 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -511,20 +505,26 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -808,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,18 +830,18 @@
       <c r="C1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="46"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="44"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="1"/>
@@ -849,10 +849,10 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -895,7 +895,7 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="40"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -906,16 +906,16 @@
       <c r="E3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="51"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="47"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="2"/>
@@ -943,10 +943,10 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="41" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -958,7 +958,7 @@
       <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="38" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="48" t="s">
@@ -977,8 +977,8 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="43"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1039,7 +1039,7 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="40" t="s">
@@ -1085,8 +1085,8 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="43"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="52" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="40" t="s">
@@ -1174,7 +1174,7 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="40"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
@@ -1218,7 +1218,7 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="52" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="40" t="s">
@@ -1230,7 +1230,9 @@
       <c r="D14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="11">
+        <v>8</v>
+      </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -1246,8 +1248,8 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
-      <c r="B15" s="43"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1290,7 +1292,7 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="52" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="40" t="s">
@@ -1320,8 +1322,8 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42"/>
-      <c r="B18" s="43"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="5" t="s">
         <v>4</v>
       </c>
@@ -1366,7 +1368,7 @@
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="39" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="40" t="s">
@@ -1406,8 +1408,8 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="51"/>
       <c r="C21" s="6" t="s">
         <v>4</v>
       </c>
@@ -1622,6 +1624,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B2:B3"/>
@@ -1631,14 +1641,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="F3:M3"/>
     <mergeCell ref="G5:M5"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed to little endian-com; Enhanced timescale at higher numbers by changing to double in chart, Added get_status
</commit_message>
<xml_diff>
--- a/doc/SPI-Protokoll.xlsx
+++ b/doc/SPI-Protokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klosskopf\Desktop\Arbeit\Messbox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7416D5-DBEC-4744-8E06-A5CD2C73BABA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D31039-3A44-4AB7-8AD1-0659C1C6E6B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7650" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
   <si>
     <t>Befehl</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>ascii</t>
-  </si>
-  <si>
-    <t>binär</t>
   </si>
   <si>
     <t>paket_size[4B]</t>
@@ -107,10 +104,6 @@
 (schreibt den Buffer, bis er voll ist)</t>
   </si>
   <si>
-    <t>Einzelner 
-Empfänger</t>
-  </si>
-  <si>
     <t>Broadcast</t>
   </si>
   <si>
@@ -183,14 +176,33 @@
     <t>wert</t>
   </si>
   <si>
-    <t>kartenname,nummer,name,typ(s/f),parametrierbar(l/f/n),min,max,plotbar(y/n){wahl1,wahl2,…};name,typ(s/f) …</t>
+    <t>Die daten werden little-Endian übertragen: =&gt; 0x12345678 wird als 0x78 -&gt; 0x56 -&gt; 0x34 -&gt; 0x12 übertragen.
+Da es sich im Falle von STM32 und Raspberry pi jeweils um little Endian Systeme handelt, liegen die Daten so im Speicher und können einfach der Reihe nach übertragen werden. Am elegantesten mittels Union; Ascii natürlich von vorne nach hinten (wie im Speicher angeordnet)</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>uint32_t</t>
+  </si>
+  <si>
+    <t>einzelne Karte</t>
+  </si>
+  <si>
+    <t>Basisplatine AVR</t>
+  </si>
+  <si>
+    <t>uint8_t</t>
+  </si>
+  <si>
+    <t>kartenname,nummer,name,typ(s/f),parametrierbar(l/f/n),min,max{wahl1,wahl2,…}nummer,name,typ(s/f) …</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +216,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +261,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -372,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -395,9 +432,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -417,9 +451,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -432,10 +463,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -469,9 +496,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -480,16 +504,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -502,30 +526,88 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -808,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,27 +903,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="44"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="39"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="1"/>
@@ -849,789 +931,792 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="E2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="62"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
+      <c r="D3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" s="28"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
+      <c r="E5" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
-      <c r="B6" s="41"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
+      <c r="D6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="28"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="33" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="E8" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="13" t="s">
+      <c r="D9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="J9" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="K9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="L9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="25"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="21"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>23</v>
+      <c r="A11" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
+      <c r="D11" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
+      <c r="D12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" s="28"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="40" t="s">
-        <v>24</v>
+      <c r="A14" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="11">
-        <v>8</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
+      <c r="D14" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
+      <c r="D15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="40" t="s">
-        <v>36</v>
+      <c r="A17" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
+      <c r="D18" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29"/>
-      <c r="B19" s="28"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="40" t="s">
-        <v>38</v>
+      <c r="A20" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>36</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
+      <c r="D20" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="64"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="36" t="s">
+      <c r="D21" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="H21" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="I21" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="J21" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="I21" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
     </row>
-    <row r="22" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
+    <row r="22" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
+    <row r="24" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="66"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="17"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
     </row>
     <row r="27" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
+  <mergeCells count="18">
+    <mergeCell ref="C23:M24"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B2:B3"/>
@@ -1641,6 +1726,14 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="F3:M3"/>
     <mergeCell ref="G5:M5"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated spi protocoll; added dummy module
</commit_message>
<xml_diff>
--- a/doc/SPI-Protokoll.xlsx
+++ b/doc/SPI-Protokoll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klosskopf\Desktop\Arbeit\Messbox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D31039-3A44-4AB7-8AD1-0659C1C6E6B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8A883E-AADC-40A0-9B55-817D817D1185}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-7650" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
   <si>
     <t>Befehl</t>
   </si>
@@ -152,9 +152,6 @@
     <t>0x09</t>
   </si>
   <si>
-    <t>samplefreq[4B]</t>
-  </si>
-  <si>
     <t>5V[4B]</t>
   </si>
   <si>
@@ -196,6 +193,15 @@
   </si>
   <si>
     <t>kartenname,nummer,name,typ(s/f),parametrierbar(l/f/n),min,max{wahl1,wahl2,…}nummer,name,typ(s/f) …</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>stopt alle Messungen</t>
+  </si>
+  <si>
+    <t>0x0A</t>
   </si>
 </sst>
 </file>
@@ -280,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -405,11 +411,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -496,24 +558,79 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -526,6 +643,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -538,76 +658,36 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -888,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,18 +992,18 @@
       <c r="C1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="39"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="58"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="1"/>
@@ -931,16 +1011,16 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="56" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="38" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -977,27 +1057,27 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="41"/>
+      <c r="F3" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="61"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="2"/>
@@ -1025,33 +1105,33 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="55" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="60" t="s">
+      <c r="F5" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="43"/>
+      <c r="G5" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="63"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="2"/>
@@ -1059,8 +1139,8 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1121,19 +1201,19 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="54" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="42" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -1167,8 +1247,8 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="53"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1178,10 +1258,10 @@
       <c r="E9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="F9" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="41" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="12" t="s">
@@ -1228,16 +1308,16 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="54" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="19"/>
@@ -1256,8 +1336,8 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1270,7 +1350,7 @@
         <v>15</v>
       </c>
       <c r="H12" s="10"/>
-      <c r="I12" s="51" t="s">
+      <c r="I12" s="34" t="s">
         <v>24</v>
       </c>
       <c r="J12" s="10"/>
@@ -1291,11 +1371,11 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="10"/>
-      <c r="I13" s="52" t="s">
-        <v>50</v>
+      <c r="I13" s="35" t="s">
+        <v>49</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -1308,26 +1388,26 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="39" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="50" t="s">
-        <v>49</v>
+      <c r="G14" s="33" t="s">
+        <v>48</v>
       </c>
       <c r="H14" s="10"/>
-      <c r="I14" s="53" t="s">
-        <v>51</v>
+      <c r="I14" s="36" t="s">
+        <v>50</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -1340,8 +1420,8 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="5" t="s">
         <v>4</v>
       </c>
@@ -1350,8 +1430,8 @@
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="54" t="s">
-        <v>52</v>
+      <c r="G15" s="37" t="s">
+        <v>51</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -1386,21 +1466,19 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="A17" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>39</v>
-      </c>
+      <c r="E17" s="19"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1416,17 +1494,15 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="5" t="s">
+      <c r="A18" s="67"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>6</v>
-      </c>
+      <c r="D18" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="19"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
@@ -1443,10 +1519,10 @@
     </row>
     <row r="19" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
-      <c r="B19" s="24"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="5"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="10"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -1462,36 +1538,24 @@
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>36</v>
+      <c r="A20" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>34</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
@@ -1502,32 +1566,20 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="64"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="6" t="s">
+      <c r="A21" s="67"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="J21" s="32" t="s">
-        <v>45</v>
-      </c>
+      <c r="D21" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="68"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
@@ -1538,6 +1590,10 @@
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -1554,21 +1610,39 @@
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="65"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="46"/>
+      <c r="A23" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
       <c r="P23" s="2"/>
@@ -1576,27 +1650,43 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="66"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="49"/>
+      <c r="A24" s="65"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
     </row>
-    <row r="25" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="15"/>
+    <row r="25" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -1612,49 +1702,64 @@
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-    </row>
-    <row r="27" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-    </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="45"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-    </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -1667,7 +1772,7 @@
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -1680,7 +1785,7 @@
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -1697,11 +1802,7 @@
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
@@ -1714,9 +1815,60 @@
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
     </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="15"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="C23:M24"/>
+  <mergeCells count="20">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C26:M27"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B2:B3"/>
@@ -1726,14 +1878,12 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="F3:M3"/>
     <mergeCell ref="G5:M5"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added DMA for data transferer, changed spi protokol
</commit_message>
<xml_diff>
--- a/doc/SPI-Protokoll.xlsx
+++ b/doc/SPI-Protokoll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klosskopf\Desktop\Arbeit\Messbox\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8A883E-AADC-40A0-9B55-817D817D1185}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EB9788-804F-49CF-B094-6744A6E13030}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,9 +149,6 @@
     <t>0x08</t>
   </si>
   <si>
-    <t>0x09</t>
-  </si>
-  <si>
     <t>5V[4B]</t>
   </si>
   <si>
@@ -201,7 +198,10 @@
     <t>stopt alle Messungen</t>
   </si>
   <si>
-    <t>0x0A</t>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>0x05</t>
   </si>
 </sst>
 </file>
@@ -607,6 +607,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -628,12 +655,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -666,27 +687,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -971,7 +971,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,18 +992,18 @@
       <c r="C1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="65"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="1"/>
@@ -1011,10 +1011,10 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="63" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="23" t="s">
@@ -1057,7 +1057,7 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53"/>
+      <c r="A3" s="62"/>
       <c r="B3" s="54"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -1068,16 +1068,16 @@
       <c r="E3" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
+      <c r="F3" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="68"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="2"/>
@@ -1105,7 +1105,7 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="62" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="55" t="s">
@@ -1123,15 +1123,15 @@
       <c r="F5" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="63"/>
+      <c r="G5" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="70"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="2"/>
@@ -1139,7 +1139,7 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="53"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="55"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
@@ -1201,7 +1201,7 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="62" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="54" t="s">
@@ -1247,7 +1247,7 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="55"/>
       <c r="C9" s="3" t="s">
         <v>4</v>
@@ -1308,7 +1308,7 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="53" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="54" t="s">
@@ -1318,7 +1318,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="10"/>
@@ -1336,7 +1336,7 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="54"/>
       <c r="C12" s="3" t="s">
         <v>4</v>
@@ -1371,11 +1371,11 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -1388,7 +1388,7 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="67" t="s">
+      <c r="A14" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="54" t="s">
@@ -1398,16 +1398,16 @@
         <v>3</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -1420,7 +1420,7 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="67"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="55"/>
       <c r="C15" s="5" t="s">
         <v>4</v>
@@ -1431,7 +1431,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -1466,17 +1466,17 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="67" t="s">
+      <c r="A17" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="70" t="s">
-        <v>37</v>
+      <c r="D17" s="49" t="s">
+        <v>31</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="10"/>
@@ -1494,12 +1494,12 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="67"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="55"/>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="50" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="19"/>
@@ -1538,7 +1538,7 @@
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="53" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="54" t="s">
@@ -1547,8 +1547,8 @@
       <c r="C20" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="72" t="s">
-        <v>38</v>
+      <c r="D20" s="51" t="s">
+        <v>32</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="10"/>
@@ -1566,15 +1566,15 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="55"/>
       <c r="C21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="68"/>
+      <c r="D21" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="47"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
@@ -1610,7 +1610,7 @@
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="71" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="54" t="s">
@@ -1620,7 +1620,7 @@
         <v>3</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>6</v>
@@ -1650,8 +1650,8 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="65"/>
-      <c r="B24" s="66"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="6" t="s">
         <v>4</v>
       </c>
@@ -1659,22 +1659,22 @@
         <v>6</v>
       </c>
       <c r="E24" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="G24" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="H24" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="30" t="s">
+      <c r="I24" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="I24" s="30" t="s">
+      <c r="J24" s="31" t="s">
         <v>43</v>
-      </c>
-      <c r="J24" s="31" t="s">
-        <v>44</v>
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
@@ -1704,19 +1704,19 @@
     <row r="26" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
-      <c r="C26" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="49"/>
+      <c r="C26" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="58"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
       <c r="P26" s="2"/>
@@ -1726,17 +1726,17 @@
     <row r="27" spans="1:18" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="45"/>
       <c r="B27" s="46"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="52"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="61"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="2"/>
@@ -1864,11 +1864,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C26:M27"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B2:B3"/>
@@ -1878,12 +1877,13 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="F3:M3"/>
     <mergeCell ref="G5:M5"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C26:M27"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>